<commit_message>
Feat: Recebendo arquivo .xlsx e .csv
</commit_message>
<xml_diff>
--- a/tabela_alunos_e_contratante.xlsx
+++ b/tabela_alunos_e_contratante.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williansantos/Documents/projetos-pessoais/automacao_planilha/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00950516-394C-0F4B-BCFE-FFBB50F66C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC061F1-2A79-0D4D-B2DB-E1987F091746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2260" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="41">
   <si>
     <t>respondent_id</t>
   </si>
@@ -526,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R32"/>
+  <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -788,104 +788,996 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="A8">
+        <v>118815909042</v>
+      </c>
+      <c r="B8">
+        <v>457453126</v>
+      </c>
+      <c r="C8" s="1">
+        <v>45723.742175925923</v>
+      </c>
+      <c r="D8" s="1">
+        <v>45723.742962962962</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q8">
+        <v>10</v>
+      </c>
+      <c r="R8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="A9">
+        <v>118815073984</v>
+      </c>
+      <c r="B9">
+        <v>457453126</v>
+      </c>
+      <c r="C9" s="1">
+        <v>45722.683229166665</v>
+      </c>
+      <c r="D9" s="1">
+        <v>45722.684062499997</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M9" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q9">
+        <v>10</v>
+      </c>
+      <c r="R9" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="A10">
+        <v>118815062940</v>
+      </c>
+      <c r="B10">
+        <v>457453126</v>
+      </c>
+      <c r="C10" s="1">
+        <v>45722.674942129626</v>
+      </c>
+      <c r="D10" s="1">
+        <v>45722.675185185188</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N10" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q10">
+        <v>10</v>
+      </c>
+      <c r="R10" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="A11">
+        <v>118815031694</v>
+      </c>
+      <c r="B11">
+        <v>457453126</v>
+      </c>
+      <c r="C11" s="1">
+        <v>45722.648993055554</v>
+      </c>
+      <c r="D11" s="1">
+        <v>45722.649699074071</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" t="s">
+        <v>35</v>
+      </c>
+      <c r="N11" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q11">
+        <v>10</v>
+      </c>
+      <c r="R11" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="A12">
+        <v>118815028681</v>
+      </c>
+      <c r="B12">
+        <v>457453126</v>
+      </c>
+      <c r="C12" s="1">
+        <v>45722.646620370368</v>
+      </c>
+      <c r="D12" s="1">
+        <v>45722.647152777776</v>
+      </c>
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12" t="s">
+        <v>38</v>
+      </c>
+      <c r="K12" t="s">
+        <v>39</v>
+      </c>
+      <c r="M12" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q12">
+        <v>9</v>
+      </c>
+      <c r="R12" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="A13">
+        <v>118815909042</v>
+      </c>
+      <c r="B13">
+        <v>457453126</v>
+      </c>
+      <c r="C13" s="1">
+        <v>45723.742175925923</v>
+      </c>
+      <c r="D13" s="1">
+        <v>45723.742962962962</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" t="s">
+        <v>23</v>
+      </c>
+      <c r="M13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q13">
+        <v>10</v>
+      </c>
+      <c r="R13" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="A14">
+        <v>118815073984</v>
+      </c>
+      <c r="B14">
+        <v>457453126</v>
+      </c>
+      <c r="C14" s="1">
+        <v>45722.683229166665</v>
+      </c>
+      <c r="D14" s="1">
+        <v>45722.684062499997</v>
+      </c>
+      <c r="E14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" t="s">
+        <v>26</v>
+      </c>
+      <c r="K14" t="s">
+        <v>27</v>
+      </c>
+      <c r="M14" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q14">
+        <v>10</v>
+      </c>
+      <c r="R14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="A15">
+        <v>118815062940</v>
+      </c>
+      <c r="B15">
+        <v>457453126</v>
+      </c>
+      <c r="C15" s="1">
+        <v>45722.674942129626</v>
+      </c>
+      <c r="D15" s="1">
+        <v>45722.675185185188</v>
+      </c>
+      <c r="E15" t="s">
+        <v>29</v>
+      </c>
+      <c r="J15" t="s">
+        <v>30</v>
+      </c>
+      <c r="K15" t="s">
+        <v>31</v>
+      </c>
+      <c r="N15" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q15">
+        <v>10</v>
+      </c>
+      <c r="R15" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
+      <c r="A16">
+        <v>118815031694</v>
+      </c>
+      <c r="B16">
+        <v>457453126</v>
+      </c>
+      <c r="C16" s="1">
+        <v>45722.648993055554</v>
+      </c>
+      <c r="D16" s="1">
+        <v>45722.649699074071</v>
+      </c>
+      <c r="E16" t="s">
+        <v>33</v>
+      </c>
+      <c r="J16" t="s">
+        <v>34</v>
+      </c>
+      <c r="K16" t="s">
+        <v>35</v>
+      </c>
+      <c r="N16" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q16">
+        <v>10</v>
+      </c>
+      <c r="R16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>118815028681</v>
+      </c>
+      <c r="B17">
+        <v>457453126</v>
+      </c>
+      <c r="C17" s="1">
+        <v>45722.646620370368</v>
+      </c>
+      <c r="D17" s="1">
+        <v>45722.647152777776</v>
+      </c>
+      <c r="E17" t="s">
+        <v>37</v>
+      </c>
+      <c r="J17" t="s">
+        <v>38</v>
+      </c>
+      <c r="K17" t="s">
+        <v>39</v>
+      </c>
+      <c r="M17" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q17">
+        <v>9</v>
+      </c>
+      <c r="R17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>118815909042</v>
+      </c>
+      <c r="B18">
+        <v>457453126</v>
+      </c>
+      <c r="C18" s="1">
+        <v>45723.742175925923</v>
+      </c>
+      <c r="D18" s="1">
+        <v>45723.742962962962</v>
+      </c>
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
+      <c r="J18" t="s">
+        <v>22</v>
+      </c>
+      <c r="K18" t="s">
+        <v>23</v>
+      </c>
+      <c r="M18" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q18">
+        <v>10</v>
+      </c>
+      <c r="R18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>118815073984</v>
+      </c>
+      <c r="B19">
+        <v>457453126</v>
+      </c>
+      <c r="C19" s="1">
+        <v>45722.683229166665</v>
+      </c>
+      <c r="D19" s="1">
+        <v>45722.684062499997</v>
+      </c>
+      <c r="E19" t="s">
+        <v>25</v>
+      </c>
+      <c r="J19" t="s">
+        <v>26</v>
+      </c>
+      <c r="K19" t="s">
+        <v>27</v>
+      </c>
+      <c r="M19" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q19">
+        <v>10</v>
+      </c>
+      <c r="R19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>118815062940</v>
+      </c>
+      <c r="B20">
+        <v>457453126</v>
+      </c>
+      <c r="C20" s="1">
+        <v>45722.674942129626</v>
+      </c>
+      <c r="D20" s="1">
+        <v>45722.675185185188</v>
+      </c>
+      <c r="E20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J20" t="s">
+        <v>30</v>
+      </c>
+      <c r="K20" t="s">
+        <v>31</v>
+      </c>
+      <c r="N20" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q20">
+        <v>10</v>
+      </c>
+      <c r="R20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>118815031694</v>
+      </c>
+      <c r="B21">
+        <v>457453126</v>
+      </c>
+      <c r="C21" s="1">
+        <v>45722.648993055554</v>
+      </c>
+      <c r="D21" s="1">
+        <v>45722.649699074071</v>
+      </c>
+      <c r="E21" t="s">
+        <v>33</v>
+      </c>
+      <c r="J21" t="s">
+        <v>34</v>
+      </c>
+      <c r="K21" t="s">
+        <v>35</v>
+      </c>
+      <c r="N21" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q21">
+        <v>10</v>
+      </c>
+      <c r="R21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>118815028681</v>
+      </c>
+      <c r="B22">
+        <v>457453126</v>
+      </c>
+      <c r="C22" s="1">
+        <v>45722.646620370368</v>
+      </c>
+      <c r="D22" s="1">
+        <v>45722.647152777776</v>
+      </c>
+      <c r="E22" t="s">
+        <v>37</v>
+      </c>
+      <c r="J22" t="s">
+        <v>38</v>
+      </c>
+      <c r="K22" t="s">
+        <v>39</v>
+      </c>
+      <c r="M22" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q22">
+        <v>9</v>
+      </c>
+      <c r="R22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>118815909042</v>
+      </c>
+      <c r="B23">
+        <v>457453126</v>
+      </c>
+      <c r="C23" s="1">
+        <v>45723.742175925923</v>
+      </c>
+      <c r="D23" s="1">
+        <v>45723.742962962962</v>
+      </c>
+      <c r="E23" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23" t="s">
+        <v>22</v>
+      </c>
+      <c r="K23" t="s">
+        <v>23</v>
+      </c>
+      <c r="M23" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q23">
+        <v>10</v>
+      </c>
+      <c r="R23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>118815073984</v>
+      </c>
+      <c r="B24">
+        <v>457453126</v>
+      </c>
+      <c r="C24" s="1">
+        <v>45722.683229166665</v>
+      </c>
+      <c r="D24" s="1">
+        <v>45722.684062499997</v>
+      </c>
+      <c r="E24" t="s">
+        <v>25</v>
+      </c>
+      <c r="J24" t="s">
+        <v>26</v>
+      </c>
+      <c r="K24" t="s">
+        <v>27</v>
+      </c>
+      <c r="M24" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q24">
+        <v>10</v>
+      </c>
+      <c r="R24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>118815062940</v>
+      </c>
+      <c r="B25">
+        <v>457453126</v>
+      </c>
+      <c r="C25" s="1">
+        <v>45722.674942129626</v>
+      </c>
+      <c r="D25" s="1">
+        <v>45722.675185185188</v>
+      </c>
+      <c r="E25" t="s">
+        <v>29</v>
+      </c>
+      <c r="J25" t="s">
+        <v>30</v>
+      </c>
+      <c r="K25" t="s">
+        <v>31</v>
+      </c>
+      <c r="N25" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q25">
+        <v>10</v>
+      </c>
+      <c r="R25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>118815031694</v>
+      </c>
+      <c r="B26">
+        <v>457453126</v>
+      </c>
+      <c r="C26" s="1">
+        <v>45722.648993055554</v>
+      </c>
+      <c r="D26" s="1">
+        <v>45722.649699074071</v>
+      </c>
+      <c r="E26" t="s">
+        <v>33</v>
+      </c>
+      <c r="J26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K26" t="s">
+        <v>35</v>
+      </c>
+      <c r="N26" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q26">
+        <v>10</v>
+      </c>
+      <c r="R26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>118815028681</v>
+      </c>
+      <c r="B27">
+        <v>457453126</v>
+      </c>
+      <c r="C27" s="1">
+        <v>45722.646620370368</v>
+      </c>
+      <c r="D27" s="1">
+        <v>45722.647152777776</v>
+      </c>
+      <c r="E27" t="s">
+        <v>37</v>
+      </c>
+      <c r="J27" t="s">
+        <v>38</v>
+      </c>
+      <c r="K27" t="s">
+        <v>39</v>
+      </c>
+      <c r="M27" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q27">
+        <v>9</v>
+      </c>
+      <c r="R27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>118815909042</v>
+      </c>
+      <c r="B28">
+        <v>457453126</v>
+      </c>
+      <c r="C28" s="1">
+        <v>45723.742175925923</v>
+      </c>
+      <c r="D28" s="1">
+        <v>45723.742962962962</v>
+      </c>
+      <c r="E28" t="s">
+        <v>21</v>
+      </c>
+      <c r="J28" t="s">
+        <v>22</v>
+      </c>
+      <c r="K28" t="s">
+        <v>23</v>
+      </c>
+      <c r="M28" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q28">
+        <v>10</v>
+      </c>
+      <c r="R28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>118815073984</v>
+      </c>
+      <c r="B29">
+        <v>457453126</v>
+      </c>
+      <c r="C29" s="1">
+        <v>45722.683229166665</v>
+      </c>
+      <c r="D29" s="1">
+        <v>45722.684062499997</v>
+      </c>
+      <c r="E29" t="s">
+        <v>25</v>
+      </c>
+      <c r="J29" t="s">
+        <v>26</v>
+      </c>
+      <c r="K29" t="s">
+        <v>27</v>
+      </c>
+      <c r="M29" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q29">
+        <v>10</v>
+      </c>
+      <c r="R29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>118815062940</v>
+      </c>
+      <c r="B30">
+        <v>457453126</v>
+      </c>
+      <c r="C30" s="1">
+        <v>45722.674942129626</v>
+      </c>
+      <c r="D30" s="1">
+        <v>45722.675185185188</v>
+      </c>
+      <c r="E30" t="s">
+        <v>29</v>
+      </c>
+      <c r="J30" t="s">
+        <v>30</v>
+      </c>
+      <c r="K30" t="s">
+        <v>31</v>
+      </c>
+      <c r="N30" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q30">
+        <v>10</v>
+      </c>
+      <c r="R30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>118815031694</v>
+      </c>
+      <c r="B31">
+        <v>457453126</v>
+      </c>
+      <c r="C31" s="1">
+        <v>45722.648993055554</v>
+      </c>
+      <c r="D31" s="1">
+        <v>45722.649699074071</v>
+      </c>
+      <c r="E31" t="s">
+        <v>33</v>
+      </c>
+      <c r="J31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K31" t="s">
+        <v>35</v>
+      </c>
+      <c r="N31" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q31">
+        <v>10</v>
+      </c>
+      <c r="R31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>118815028681</v>
+      </c>
+      <c r="B32">
+        <v>457453126</v>
+      </c>
+      <c r="C32" s="1">
+        <v>45722.646620370368</v>
+      </c>
+      <c r="D32" s="1">
+        <v>45722.647152777776</v>
+      </c>
+      <c r="E32" t="s">
+        <v>37</v>
+      </c>
+      <c r="J32" t="s">
+        <v>38</v>
+      </c>
+      <c r="K32" t="s">
+        <v>39</v>
+      </c>
+      <c r="M32" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q32">
+        <v>9</v>
+      </c>
+      <c r="R32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>118815909042</v>
+      </c>
+      <c r="B35">
+        <v>457453126</v>
+      </c>
+      <c r="C35" s="1">
+        <v>45723.742175925923</v>
+      </c>
+      <c r="D35" s="1">
+        <v>45723.742962962962</v>
+      </c>
+      <c r="E35" t="s">
+        <v>21</v>
+      </c>
+      <c r="J35" t="s">
+        <v>22</v>
+      </c>
+      <c r="K35" t="s">
+        <v>23</v>
+      </c>
+      <c r="M35" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q35">
+        <v>10</v>
+      </c>
+      <c r="R35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>118815073984</v>
+      </c>
+      <c r="B36">
+        <v>457453126</v>
+      </c>
+      <c r="C36" s="1">
+        <v>45722.683229166665</v>
+      </c>
+      <c r="D36" s="1">
+        <v>45722.684062499997</v>
+      </c>
+      <c r="E36" t="s">
+        <v>25</v>
+      </c>
+      <c r="J36" t="s">
+        <v>26</v>
+      </c>
+      <c r="K36" t="s">
+        <v>27</v>
+      </c>
+      <c r="M36" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q36">
+        <v>10</v>
+      </c>
+      <c r="R36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>118815062940</v>
+      </c>
+      <c r="B37">
+        <v>457453126</v>
+      </c>
+      <c r="C37" s="1">
+        <v>45722.674942129626</v>
+      </c>
+      <c r="D37" s="1">
+        <v>45722.675185185188</v>
+      </c>
+      <c r="E37" t="s">
+        <v>29</v>
+      </c>
+      <c r="J37" t="s">
+        <v>30</v>
+      </c>
+      <c r="K37" t="s">
+        <v>31</v>
+      </c>
+      <c r="N37" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q37">
+        <v>10</v>
+      </c>
+      <c r="R37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>118815031694</v>
+      </c>
+      <c r="B38">
+        <v>457453126</v>
+      </c>
+      <c r="C38" s="1">
+        <v>45722.648993055554</v>
+      </c>
+      <c r="D38" s="1">
+        <v>45722.649699074071</v>
+      </c>
+      <c r="E38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J38" t="s">
+        <v>34</v>
+      </c>
+      <c r="K38" t="s">
+        <v>35</v>
+      </c>
+      <c r="N38" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q38">
+        <v>10</v>
+      </c>
+      <c r="R38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>118815028681</v>
+      </c>
+      <c r="B39">
+        <v>457453126</v>
+      </c>
+      <c r="C39" s="1">
+        <v>45722.646620370368</v>
+      </c>
+      <c r="D39" s="1">
+        <v>45722.647152777776</v>
+      </c>
+      <c r="E39" t="s">
+        <v>37</v>
+      </c>
+      <c r="J39" t="s">
+        <v>38</v>
+      </c>
+      <c r="K39" t="s">
+        <v>39</v>
+      </c>
+      <c r="M39" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q39">
+        <v>9</v>
+      </c>
+      <c r="R39" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>118815028681</v>
+      </c>
+      <c r="B40">
+        <v>457453126</v>
+      </c>
+      <c r="C40" s="1">
+        <v>45722.646620370368</v>
+      </c>
+      <c r="D40" s="1">
+        <v>45722.647152777776</v>
+      </c>
+      <c r="E40" t="s">
+        <v>37</v>
+      </c>
+      <c r="J40" t="s">
+        <v>38</v>
+      </c>
+      <c r="K40" t="s">
+        <v>39</v>
+      </c>
+      <c r="M40" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q40">
+        <v>9</v>
+      </c>
+      <c r="R40" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>